<commit_message>
implementation of api to get recommendation
</commit_message>
<xml_diff>
--- a/history.xlsx
+++ b/history.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -670,7 +670,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>45729.4858264516</v>
+        <v>45729.48582644676</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -756,6 +756,180 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" s="2" t="n">
+        <v>45729.49783483797</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Aarti</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>25</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>50</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G5" t="n">
+        <v>22.22</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Normal weight - Maintain a balanced diet and exercise.</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Veg</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>calcium</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Recommendations for calcium Deficiency:
+Tofu, raw, firm, prepared with calcium sulfate
+Cheese, Mexican, blend, reduced fat
+Cheese, cheddar, nonfat or fat free
+Cheese, swiss, low fat
+Cheese, swiss, low sodium
+Cheese, mozzarella, part skim milk
+Cheese, gruyere
+Cheese, monterey
+Cheese, port de salut
+Cheese, swiss
+Cheese, swiss
+Cheese, provolone, sliced
+Cheese, provolone, reduced fat
+Cheese, monterey jack, solid
+Cheese, low-sodium, cheddar or colby
+Cheese, muenster
+Cheese, mozzarella, low sodium
+Cheese, provolone
+Cheese, monterey, low fat
+Cheese, brick
+Cheese, mexican, queso asadero
+Cheese, colby
+Cheese, Mexican blend
+Cheese, Swiss, nonfat or fat free
+Cheese, queso fresco, solid
+Cheese, cheddar
+Cheese, mexican, queso chihuahua
+Cheese, cheddar, sharp, sliced
+Cheese, cheddar
+Cheese, white, queso blanco
+Cheese, mozzarella, nonfat
+Cheese, cheddar, reduced fat
+Cheese, tilsit
+Cheese, parmesan, grated, refrigerated
+Cheese, cheshire
+Cheese, parmesan, hard
+Cheese, caraway
+Imitation cheese, american or cheddar, low cholesterol
+Cheese, fontina
+Cheese, mexican, queso anejo</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="n">
+        <v>45729.51109761735</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Aarti</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>25</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>50</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G6" t="n">
+        <v>22.22</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Normal weight - Maintain a balanced diet and exercise.</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Veg</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>calcium, vitamin_E</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Recommendations for calcium and vitamin_E Deficiency:
+Cheese, swiss
+Cheese, swiss
+Cheese, cheddar, sharp, sliced
+Cheese, Mexican, blend, reduced fat
+Grape leaves, raw
+Cheese, cheddar
+Cheese, swiss, low sodium
+Cheese, cheddar
+Tofu, raw, firm, prepared with calcium sulfate
+Cheese, gruyere
+Cheese, monterey
+Turnip greens, raw
+Cheese, port de salut
+Cheese, mozzarella, part skim milk
+Cheese, cheddar, nonfat or fat free
+Cheese, white, queso blanco
+Cheese, swiss, low fat
+Cheese, cheddar, reduced fat
+Cheese, low-sodium, cheddar or colby
+Cheese, muenster
+Peppers, jalapeno, raw
+Cheese, provolone
+Cheese, colby
+Cheese, brick
+Cheese, provolone, reduced fat
+Cheese, mexican, queso asadero
+Cheese, Mexican blend
+Cheese, monterey, low fat
+Cheese, mexican, queso chihuahua
+Cheese, mozzarella, low sodium
+Cheese, mozzarella, low moisture, part-skim, shredded
+Cheese, mozzarella, low moisture, part-skim
+Cheese food, pasteurized process, American, vitamin D fortified
+Cheese, pasteurized process, American, without added vitamin D
+Cheese, provolone, sliced
+Cheese, mozzarella, low moisture, part-skim
+Cheese product, pasteurized process, American, vitamin D fortified
+Cheese, monterey jack, solid</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
changed post getrecommendation api to get
</commit_message>
<xml_diff>
--- a/history.xlsx
+++ b/history.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -846,7 +846,7 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>45729.51109761735</v>
+        <v>45729.51109761574</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -930,6 +930,270 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" s="2" t="n">
+        <v>45730.43464201389</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Aarti</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>25</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>50</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G7" t="n">
+        <v>22.22</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Normal weight - Maintain a balanced diet and exercise.</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Veg</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>calcium</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Recommendations for calcium Deficiency:
+Tofu, raw, firm, prepared with calcium sulfate
+Cheese, Mexican, blend, reduced fat
+Cheese, cheddar, nonfat or fat free
+Cheese, swiss, low fat
+Cheese, swiss, low sodium
+Cheese, mozzarella, part skim milk
+Cheese, gruyere
+Cheese, monterey
+Cheese, port de salut
+Cheese, swiss
+Cheese, swiss
+Cheese, provolone, sliced
+Cheese, provolone, reduced fat
+Cheese, monterey jack, solid
+Cheese, low-sodium, cheddar or colby
+Cheese, muenster
+Cheese, mozzarella, low sodium
+Cheese, provolone
+Cheese, monterey, low fat
+Cheese, brick
+Cheese, mexican, queso asadero
+Cheese, colby
+Cheese, Mexican blend
+Cheese, Swiss, nonfat or fat free
+Cheese, queso fresco, solid
+Cheese, cheddar
+Cheese, mexican, queso chihuahua
+Cheese, cheddar, sharp, sliced
+Cheese, cheddar
+Cheese, white, queso blanco
+Cheese, mozzarella, nonfat
+Cheese, cheddar, reduced fat
+Cheese, tilsit
+Cheese, parmesan, grated, refrigerated
+Cheese, cheshire
+Cheese, parmesan, hard
+Cheese, caraway
+Imitation cheese, american or cheddar, low cholesterol
+Cheese, fontina
+Cheese, mexican, queso anejo</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="n">
+        <v>45730.43493046296</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Aarti</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>25</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>50</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G8" t="n">
+        <v>22.22</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Normal weight - Maintain a balanced diet and exercise.</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Veg</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>calcium</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Recommendations for calcium Deficiency:
+Tofu, raw, firm, prepared with calcium sulfate
+Cheese, Mexican, blend, reduced fat
+Cheese, cheddar, nonfat or fat free
+Cheese, swiss, low fat
+Cheese, swiss, low sodium
+Cheese, mozzarella, part skim milk
+Cheese, gruyere
+Cheese, monterey
+Cheese, port de salut
+Cheese, swiss
+Cheese, swiss
+Cheese, provolone, sliced
+Cheese, provolone, reduced fat
+Cheese, monterey jack, solid
+Cheese, low-sodium, cheddar or colby
+Cheese, muenster
+Cheese, mozzarella, low sodium
+Cheese, provolone
+Cheese, monterey, low fat
+Cheese, brick
+Cheese, mexican, queso asadero
+Cheese, colby
+Cheese, Mexican blend
+Cheese, Swiss, nonfat or fat free
+Cheese, queso fresco, solid
+Cheese, cheddar
+Cheese, mexican, queso chihuahua
+Cheese, cheddar, sharp, sliced
+Cheese, cheddar
+Cheese, white, queso blanco
+Cheese, mozzarella, nonfat
+Cheese, cheddar, reduced fat
+Cheese, tilsit
+Cheese, parmesan, grated, refrigerated
+Cheese, cheshire
+Cheese, parmesan, hard
+Cheese, caraway
+Imitation cheese, american or cheddar, low cholesterol
+Cheese, fontina
+Cheese, mexican, queso anejo</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="n">
+        <v>45730.43550134636</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Aarti</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>25</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>50</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G9" t="n">
+        <v>22.22</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Normal weight - Maintain a balanced diet and exercise.</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Veg</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>calcium</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Recommendations for calcium Deficiency:
+Tofu, raw, firm, prepared with calcium sulfate
+Cheese, Mexican, blend, reduced fat
+Cheese, cheddar, nonfat or fat free
+Cheese, swiss, low fat
+Cheese, swiss, low sodium
+Cheese, mozzarella, part skim milk
+Cheese, gruyere
+Cheese, monterey
+Cheese, port de salut
+Cheese, swiss
+Cheese, swiss
+Cheese, provolone, sliced
+Cheese, provolone, reduced fat
+Cheese, monterey jack, solid
+Cheese, low-sodium, cheddar or colby
+Cheese, muenster
+Cheese, mozzarella, low sodium
+Cheese, provolone
+Cheese, monterey, low fat
+Cheese, brick
+Cheese, mexican, queso asadero
+Cheese, colby
+Cheese, Mexican blend
+Cheese, Swiss, nonfat or fat free
+Cheese, queso fresco, solid
+Cheese, cheddar
+Cheese, mexican, queso chihuahua
+Cheese, cheddar, sharp, sliced
+Cheese, cheddar
+Cheese, white, queso blanco
+Cheese, mozzarella, nonfat
+Cheese, cheddar, reduced fat
+Cheese, tilsit
+Cheese, parmesan, grated, refrigerated
+Cheese, cheshire
+Cheese, parmesan, hard
+Cheese, caraway
+Imitation cheese, american or cheddar, low cholesterol
+Cheese, fontina
+Cheese, mexican, queso anejo</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Classify recipe dataset to veg/non veg
</commit_message>
<xml_diff>
--- a/history.xlsx
+++ b/history.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1108,7 +1108,7 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>45730.43550134636</v>
+        <v>45730.4355013426</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -1194,6 +1194,271 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" s="2" t="n">
+        <v>45730.50495601852</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>fff</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>25</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>50</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G10" t="n">
+        <v>22.22</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Normal weight - Maintain a balanced diet and exercise.</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Veg</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>vitamin_C</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Recommendations for vitamin_C Deficiency:
+Acerola, (west indian cherry), raw
+Acerola juice, raw
+Guavas, common, raw
+Peppers, hot chili, green, raw
+Peppers, sweet, yellow, raw
+Mango, Ataulfo, peeled, raw
+Currants, european black, raw
+Kiwifruit, ZESPRI SunGold, raw
+Peppers, bell, orange, raw
+Drumstick pods, raw
+Pokeberry shoots, (poke), raw
+Lemon peel, raw
+Peppers, bell, yellow, raw
+Peppers, bell, red, raw
+Orange peel, raw
+Longans, raw
+Peppers, bell, green, raw
+Balsam-pear (bitter gourd), pods, raw
+Peppers, sweet, red, raw
+Litchis, raw
+Broccoli, flower clusters, raw
+Broccoli, leaves, raw
+Broccoli, stalks, raw
+Jujube, raw
+Kiwifruit, green, raw
+Peppers, sweet, green, raw
+Persimmons, native, raw
+Taro, tahitian, raw
+Pummelo, raw
+Strawberries, raw
+Oranges, raw, with peel
+Papayas, raw
+Strawberries, raw
+Broccoli, raw
+Kiwifruit (kiwi), green, peeled, raw
+Mustard spinach, (tendergreen), raw
+Pineapple, raw
+Cauliflower, green, raw</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="n">
+        <v>45732.90905953704</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>eddc</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>25</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>50</v>
+      </c>
+      <c r="F11" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G11" t="n">
+        <v>22.22</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Normal weight - Maintain a balanced diet and exercise.</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Non-veg</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>vitamin_C</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+ Fruit
+  - Acerola, (west indian cherry), raw
+  - Guavas, common, raw
+  - Mango, Ataulfo, peeled, raw
+  - Currants, european black, raw
+  - Kiwifruit, ZESPRI SunGold, raw
+  - Lemon peel, raw
+  - Orange peel, raw
+  - Longans, raw
+  - Litchis, raw
+  - Jujube, raw
+  - Kiwifruit, green, raw
+  - Persimmons, native, raw
+  - Pummelo, raw
+  - Strawberries, raw
+  - Oranges, raw, with peel
+  - Papayas, raw
+  - Strawberries, raw
+  - Kiwifruit (kiwi), green, peeled, raw
+  - Pineapple, raw
+ Juice
+  - Acerola juice, raw
+ Non Alcoholic
+  - Beverages, tea, green, instant, decaffeinated, lemon, unsweetened, fortified with vitamin C
+  - Beverages, tea, instant, lemon, with added ascorbic acid
+ Vegetable
+  - Peppers, hot chili, green, raw
+  - Peppers, sweet, yellow, raw
+  - Peppers, bell, orange, raw
+  - Drumstick pods, raw
+  - Pokeberry shoots, (poke), raw
+  - Peppers, bell, yellow, raw
+  - Peppers, bell, red, raw
+  - Peppers, bell, green, raw
+  - Balsam-pear (bitter gourd), pods, raw
+  - Peppers, sweet, red, raw
+  - Broccoli, flower clusters, raw
+  - Broccoli, leaves, raw
+  - Broccoli, stalks, raw
+  - Peppers, sweet, green, raw
+  - Taro, tahitian, raw
+  - Broccoli, raw
+  - Mustard spinach, (tendergreen), raw
+  - Cauliflower, green, raw</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="n">
+        <v>45733.4061382423</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>25</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>50</v>
+      </c>
+      <c r="F12" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G12" t="n">
+        <v>22.22</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Normal weight - Maintain a balanced diet and exercise.</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Veg</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>vitamin_C</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+ Fruit
+  - Acerola, (west indian cherry), raw
+  - Guavas, common, raw
+  - Mango, Ataulfo, peeled, raw
+  - Currants, european black, raw
+  - Kiwifruit, ZESPRI SunGold, raw
+  - Lemon peel, raw
+  - Orange peel, raw
+  - Longans, raw
+  - Litchis, raw
+  - Jujube, raw
+  - Kiwifruit, green, raw
+  - Persimmons, native, raw
+  - Pummelo, raw
+  - Strawberries, raw
+  - Oranges, raw, with peel
+  - Papayas, raw
+  - Strawberries, raw
+  - Kiwifruit (kiwi), green, peeled, raw
+  - Pineapple, raw
+ Juice
+  - Acerola juice, raw
+ Vegetable
+  - Peppers, hot chili, green, raw
+  - Peppers, sweet, yellow, raw
+  - Peppers, bell, orange, raw
+  - Drumstick pods, raw
+  - Pokeberry shoots, (poke), raw
+  - Peppers, bell, yellow, raw
+  - Peppers, bell, red, raw
+  - Peppers, bell, green, raw
+  - Balsam-pear (bitter gourd), pods, raw
+  - Peppers, sweet, red, raw
+  - Broccoli, flower clusters, raw
+  - Broccoli, leaves, raw
+  - Broccoli, stalks, raw
+  - Peppers, sweet, green, raw
+  - Taro, tahitian, raw
+  - Broccoli, raw
+  - Mustard spinach, (tendergreen), raw
+  - Cauliflower, green, raw</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
converting notebook to py files
</commit_message>
<xml_diff>
--- a/history.xlsx
+++ b/history.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1373,7 +1373,7 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>45733.4061382423</v>
+        <v>45733.40613824074</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -1459,6 +1459,379 @@
         </is>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" s="2" t="n">
+        <v>45733.894671875</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>sasa</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>25</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>50</v>
+      </c>
+      <c r="F13" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G13" t="n">
+        <v>22.22</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Normal weight - Maintain a balanced diet and exercise.</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Veg</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>potassium</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+ Cream
+  - Cream substitute, powdered, light
+  - Cream substitute, powdered
+ Vegetable
+  - Hearts of palm, raw
+  - Yam, raw
+  - Arrowhead, raw
+  - Butterbur, (fuki), raw
+  - Yautia (tannier), raw
+  - Taro, tahitian, raw
+  - Sweet potatoes, orange flesh, without skin, raw
+  - Brussels sprouts, raw
+  - Lemon grass (citronella), raw
+  - Potatoes, red, without skin, raw
+  - Purslane, raw
+  - Potatoes, gold, without skin, raw
+  - Squash, zucchini, baby, raw
+  - Potatoes, russet, without skin, raw
+  - Potatoes, red, flesh and skin, raw
+  - Lotus root, raw
+  - Bamboo shoots, raw
+  - Drumstick pods, raw
+  - Fennel, bulb, raw
+  - Borage, raw
+  - Mountain yam, hawaii, raw
+  - Ginger root, raw
+  - Cornsalad, raw
+  - Beets, raw
+  - Wasabi, root, raw
+  - Waterchestnuts, chinese, (matai), raw
+ Nuts
+  - Seeds, breadnut tree seeds, raw
+ Fruit
+  - Breadfruit, raw
+  - Avocado, Hass, peeled, raw
+  - Plantains, yellow, raw
+  - Plantains, green, raw
+  - Plantains, underripe, raw
+  - Plantains, overripe, raw
+  - Plantains, ripe, raw</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="n">
+        <v>45733.89500943287</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>sasa</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>25</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>50</v>
+      </c>
+      <c r="F14" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G14" t="n">
+        <v>22.22</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Normal weight - Maintain a balanced diet and exercise.</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Non-veg</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>potassium</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+ Non Alcoholic
+  - Beverages, tea, instant, lemon, unsweetened
+  - Beverages, tea, instant, decaffeinated, lemon, diet
+  - Beverages, tea, instant, unsweetened, powder
+  - Beverages, coffee and cocoa, instant, decaffeinated, with whitener and low calorie sweetener
+ Cream
+  - Cream substitute, powdered, light
+  - Cream substitute, powdered
+ Vegetable
+  - Hearts of palm, raw
+  - Yam, raw
+  - Arrowhead, raw
+  - Butterbur, (fuki), raw
+  - Yautia (tannier), raw
+  - Taro, tahitian, raw
+  - Sweet potatoes, orange flesh, without skin, raw
+  - Brussels sprouts, raw
+  - Lemon grass (citronella), raw
+  - Potatoes, red, without skin, raw
+  - Purslane, raw
+  - Potatoes, gold, without skin, raw
+  - Squash, zucchini, baby, raw
+  - Potatoes, russet, without skin, raw
+  - Potatoes, red, flesh and skin, raw
+  - Lotus root, raw
+  - Bamboo shoots, raw
+  - Drumstick pods, raw
+  - Fennel, bulb, raw
+  - Borage, raw
+  - Mountain yam, hawaii, raw
+  - Ginger root, raw
+  - Cornsalad, raw
+  - Beets, raw
+  - Wasabi, root, raw
+  - Waterchestnuts, chinese, (matai), raw
+ Nuts
+  - Seeds, breadnut tree seeds, raw
+ Fruit
+  - Breadfruit, raw
+  - Avocado, Hass, peeled, raw
+  - Plantains, yellow, raw
+  - Plantains, green, raw
+  - Plantains, underripe, raw
+  - Plantains, overripe, raw
+  - Plantains, ripe, raw</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="n">
+        <v>45733.89519628472</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>sasa</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>25</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>50</v>
+      </c>
+      <c r="F15" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G15" t="n">
+        <v>22.22</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Normal weight - Maintain a balanced diet and exercise.</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Non-veg</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>potassium, sodium</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+ Pork
+  - Pork, cured, salt pork, raw
+  - Pork, cured, ham, center slice, country-style, separable lean only, raw
+  - Pork, cured, breakfast strips, raw or unheated
+  - Sausage, pork, chorizo, link or ground, raw
+  - Bockwurst, pork, veal, raw
+  - Sausage, Italian, pork, mild, raw
+ Egg
+  - Egg, whole, raw, frozen, salted, pasteurized
+ Non Alcoholic
+  - Beverages, tea, instant, decaffeinated, lemon, diet
+  - Beverages, tea, instant, lemon, unsweetened
+  - Beverages, coffee and cocoa, instant, decaffeinated, with whitener and low calorie sweetener
+  - Beverages, tea, instant, unsweetened, powder
+ Beef
+  - Beef, cured, corned beef, brisket, raw
+  - Beef, cured, breakfast strips, raw or unheated
+ Cheese
+  - Cheese, American, restaurant
+  - Cheese, roquefort
+  - Cheese, dry white, queso seco
+  - Cheese, dry white, queso seco
+  - Cheese, feta, whole milk, crumbled
+  - Cheese, blue
+  - Cheese food, pasteurized process, American, without added vitamin D
+  - Cheese, cotija, solid
+  - Cheese food, cold pack, American
+  - Cheese food, pasteurized process, swiss
+  - Cheese food, pasteurized process, American, vitamin D fortified
+  - Cheese, brie
+  - Cheese, camembert
+ Cream
+  - Cream substitute, powdered, light
+ Fish
+  - Crustaceans, crab, alaska king, raw
+  - Crustaceans, shrimp, farm raised, raw
+  - Mollusks, clam, mixed species, raw
+ Turkey
+  - Sausage, turkey, breakfast links, mild, raw
+  - Turkey roast, boneless, frozen, seasoned, light and dark meat, raw
+  - Sausage, turkey, breakfast links, mild, raw
+  - Sausage, turkey, fresh, raw
+ Vegetable
+  - Seaweed, wakame, raw
+  - Hearts of palm, raw
+ Butter
+  - Butter, whipped, with salt
+  - Butter, stick, salted
+  - Butter, salted
+ Nuts
+  - Seeds, breadnut tree seeds, raw</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="n">
+        <v>45733.89527798499</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>sasa</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>25</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>50</v>
+      </c>
+      <c r="F16" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G16" t="n">
+        <v>22.22</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Normal weight - Maintain a balanced diet and exercise.</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Non-veg</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>sodium</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+ Pork
+  - Pork, cured, salt pork, raw
+  - Pork, cured, ham, center slice, country-style, separable lean only, raw
+  - Pork, cured, breakfast strips, raw or unheated
+  - Sausage, pork, chorizo, link or ground, raw
+  - Sausage, Italian, pork, mild, raw
+  - Bockwurst, pork, veal, raw
+ Egg
+  - Egg, whole, raw, frozen, salted, pasteurized
+ Beef
+  - Beef, cured, corned beef, brisket, raw
+  - Beef, cured, breakfast strips, raw or unheated
+ Cheese
+  - Cheese, American, restaurant
+  - Cheese, roquefort
+  - Cheese, dry white, queso seco
+  - Cheese, dry white, queso seco
+  - Cheese, feta, whole milk, crumbled
+  - Cheese, cotija, solid
+  - Cheese, blue
+  - Cheese food, pasteurized process, American, without added vitamin D
+  - Cheese, brie
+  - Cheese spread, cream cheese base
+  - Cheese food, pasteurized process, swiss
+  - Cheese, camembert
+  - Cheese, cottage, lowfat, 1% milkfat, with vegetables
+  - Cheese, cottage, with vegetables
+  - Cheese, cottage, lowfat, 1% milkfat
+  - Cheese food, cold pack, American
+  - Cheese, feta
+  - Cheese food, pasteurized process, American, vitamin D fortified
+ Fish
+  - Crustaceans, crab, alaska king, raw
+  - Mollusks, clam, mixed species, raw
+  - Crustaceans, shrimp, farm raised, raw
+  - Crustaceans, crab, queen, raw
+  - Crustaceans, shrimp, mixed species, raw (may contain additives to retain moisture)
+ Vegetable
+  - Seaweed, wakame, raw
+ Butter
+  - Butter, whipped, with salt
+  - Butter, stick, salted
+  - Butter, salted
+ Turkey
+  - Sausage, turkey, breakfast links, mild, raw
+  - Turkey roast, boneless, frozen, seasoned, light and dark meat, raw
+  - Sausage, turkey, breakfast links, mild, raw
+ Cream
+  - Cream cheese, full fat, block</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>